<commit_message>
Add the workstations data analysis and update labels.xlsx
</commit_message>
<xml_diff>
--- a/data/labels.xlsx
+++ b/data/labels.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fronchettl\Documents\GitHub\workstations\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFCDD8E-7C38-4EBC-9326-64914B72ABA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Labels" sheetId="1" r:id="rId4"/>
+    <sheet name="Labels" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>Desk (Standing)</t>
   </si>
@@ -293,21 +302,44 @@
   </si>
   <si>
     <t>Notebook</t>
+  </si>
+  <si>
+    <t>Most common items, fix items instead of being occurrences, count only per person</t>
+  </si>
+  <si>
+    <t>Use our categorical data not our overall data (Amazon categories)</t>
+  </si>
+  <si>
+    <t>Doing the monitor thing including laptop (Analyze images)</t>
+  </si>
+  <si>
+    <t>Mice and keyboards as separate things</t>
+  </si>
+  <si>
+    <t>Count number of people that have at least one ergonomic item (mice, keyboard, standing desk, footrest, gaming chair, monitor arm, laptop stand, acoustic foam)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -315,7 +347,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -349,47 +381,56 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -579,24 +620,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="38.86"/>
-    <col customWidth="1" min="2" max="2" width="28.43"/>
+    <col min="1" max="1" width="38.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="7" max="7" width="133.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,466 +651,565 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="B11" s="3"/>
+      <c r="G11" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="B12" s="3"/>
+      <c r="G12" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="B13" s="3"/>
+      <c r="G13" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="B14" s="3"/>
+      <c r="G14" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="B15" s="3"/>
+      <c r="G15" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A50" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A51" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A52" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A57" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A58" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A59" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A61" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A62" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A63" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A64" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A65" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A66" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A67" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A68" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A69" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A70" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A71" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A72" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="73">
+      <c r="B72" s="3"/>
+    </row>
+    <row r="73" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="74">
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="76">
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="77">
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="78">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="79">
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="80">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="81" ht="15.0" customHeight="1">
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="82">
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="83">
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B83" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="85">
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="86">
+      <c r="B85" s="3"/>
+    </row>
+    <row r="86" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="87">
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="88">
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="89">
+      <c r="B88" s="3"/>
+    </row>
+    <row r="89" spans="1:2" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="B89" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B1:B25"/>
-    <mergeCell ref="B26:B38"/>
-    <mergeCell ref="B39:B73"/>
+    <mergeCell ref="B26:B37"/>
+    <mergeCell ref="B38:B73"/>
     <mergeCell ref="B74:B82"/>
     <mergeCell ref="B83:B89"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>